<commit_message>
BOM.xlsx updated (unknown reason)
</commit_message>
<xml_diff>
--- a/hardware-data/BOM.xlsx
+++ b/hardware-data/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="30960" windowHeight="21660" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="30960" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ICs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="195">
   <si>
     <t>Part</t>
   </si>
@@ -660,6 +660,21 @@
   </si>
   <si>
     <t>Fairchild_MM74HC245A.pdf</t>
+  </si>
+  <si>
+    <t>JP401</t>
+  </si>
+  <si>
+    <t>LH7A400 T1</t>
+  </si>
+  <si>
+    <t>LH7A400 T9</t>
+  </si>
+  <si>
+    <t>JP402</t>
+  </si>
+  <si>
+    <t>Jumper</t>
   </si>
 </sst>
 </file>
@@ -988,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1749,10 +1764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,6 +1918,28 @@
         <v>29</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>